<commit_message>
50% betere pie chart
</commit_message>
<xml_diff>
--- a/Opleverset/Extra documenten/Excel sheets/leerdoelenproces.xlsx
+++ b/Opleverset/Extra documenten/Excel sheets/leerdoelenproces.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyril\Desktop\Project-5-6---Floating-Farm\Opleverset\Extra documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyril\Desktop\Project-5-6---Floating-Farm\Opleverset\Extra documenten\Excel sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A7F2E70-6368-4DDF-9EA1-92C5CFBBF456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3ECBD9A-35A9-4A1D-AF15-FCF2E8917A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{22501029-C1EF-405D-A741-1A6A9BE757DD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>gedaan</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>totaal</t>
   </si>
 </sst>
 </file>
@@ -138,6 +141,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1AA6-482F-90F4-9D6EACC11F96}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -153,6 +161,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1AA6-482F-90F4-9D6EACC11F96}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -268,7 +281,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$18:$D$18</c:f>
+              <c:f>Blad1!$B$3:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1305,7 +1318,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1332,17 +1345,25 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <f>SUM(B4:B18)</f>
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <f>SUM(C4:C18)</f>
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <f>SUM(D4:D18)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>1+A3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1350,17 +1371,17 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" ref="A5:A17" si="0">1+A4</f>
-        <v>3</v>
-      </c>
-      <c r="C5">
+        <f>1+A4</f>
+        <v>2</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" ref="A6:A18" si="0">1+A5</f>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1369,52 +1390,52 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="B8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="D9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="B10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="C11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1423,16 +1444,16 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1440,8 +1461,8 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f>1+A14</f>
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1449,34 +1470,29 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
+        <f>1+A15</f>
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <f>SUM(B3:B17)</f>
-        <v>4</v>
-      </c>
       <c r="C18">
-        <f t="shared" ref="C18:D18" si="1">SUM(C3:C17)</f>
-        <v>8</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>